<commit_message>
Asset list tot nu toe
</commit_message>
<xml_diff>
--- a/Algemeen/Asset_List_Ninja_Breakout.xlsx
+++ b/Algemeen/Asset_List_Ninja_Breakout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$F$604</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ID Code</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t xml:space="preserve">Alert, Door, Clock, Katana Use/Hit, Charge, Climbing, Finisher, </t>
+  </si>
+  <si>
+    <t>Buttons, Scrollwheels, Dropdowns, Background</t>
+  </si>
+  <si>
+    <t>ShurikenElectriciteit, ShurikenMetal, Relics, OnHIt, Jump/Landing, GettingHit, Walking, Blood, Smoke, Rain, WaterDrops,</t>
   </si>
 </sst>
 </file>
@@ -659,7 +665,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,7 +1006,9 @@
       <c r="H15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1154,7 +1162,9 @@
       <c r="H23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>

</xml_diff>

<commit_message>
Asset list done for now
</commit_message>
<xml_diff>
--- a/Algemeen/Asset_List_Ninja_Breakout.xlsx
+++ b/Algemeen/Asset_List_Ninja_Breakout.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>ID Code</t>
   </si>
@@ -121,34 +121,46 @@
     <t>BuildingOne, BuildingTwo, Building FloorOne, Building FloorTwo, Shops, Electricity Cable, Wolken, Back BuildingOne, Back BuildingTwo,</t>
   </si>
   <si>
-    <t xml:space="preserve">Sakura Tree, TR BonsaiTree, </t>
-  </si>
-  <si>
     <t>TR Vase, TR Plants, TR Doors, TR Carpet, TR DisplayCase, TR Food, TR Lamps, TR Clock, FireExtinguisher, StreetLamps, Cars, Pavement, Moon,</t>
   </si>
   <si>
     <t xml:space="preserve">Shuriken Throw/Hitsound, Ambient City, Ambient Jail, Ambient Sewage, Ninja Girl Footsteps, Enemy Footsteps, Enemy Talking, Glass Shatter, </t>
   </si>
   <si>
-    <t>Buttons, Scrollwheels, Dropdowns, Background</t>
-  </si>
-  <si>
     <t>JailBars, JailBed, JailSink, JailToilet, Crates, Manhole, JailChair, JailDude, TLLamps, CellDoor, Boxes, GuardTable, GuardChair, PlayCards,</t>
-  </si>
-  <si>
-    <t>Alert, Door, Clock, Katana Use/Hit, Charge, Climbing, Finisher, Background</t>
   </si>
   <si>
     <t xml:space="preserve">PlayerMovement, EnemyBehaviour, PlayerAttack, Detection, Flashlight, Stealth, Environment, BossBehaviour, Events, StartMenu, InGameMenu, </t>
   </si>
   <si>
-    <t xml:space="preserve">HUD, Checkpoints, Respawn, FastTravel, </t>
+    <t>Radio, Cameras, ClothingRack, ClothingHang, JailFloor, Basketball, CourtyardBack, JailBack, HeistBack, SewageBack, ArmorPieces,</t>
   </si>
   <si>
-    <t>ShurikenElectriciteit, ShurikenMetal, Relics, OnHIt, Jump/Landing, GettingHit, Walking, Blood, Smoke, Rain, WaterDrops, Sparks</t>
+    <t>ShurikenElectriciteit, ShurikenMetal, Relics, OnHIt, Jump/Landing, GettingHit, Walking, Blood, Smoke, Rain, WaterDrops, Sparks, Steam</t>
   </si>
   <si>
-    <t xml:space="preserve">Radio, Cameras, ClothingRack, ClothingHang, JailFloor, Basketball, CourtyardBack, </t>
+    <t xml:space="preserve">WardenDesk, WardenShelf, WardenChair, WardenBack, WardenLamp, WardenAccessories, BoilerBack, Boilers, BrokenCrates, Valves, </t>
+  </si>
+  <si>
+    <t>SewerPipes, Water, SewageWaterJunk, Rats, Bird, SewageJunk, SewageLamps, SewageObstacles, SewagePlank, Cardbord, SewageProps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swimming, </t>
+  </si>
+  <si>
+    <t>Buttons, Scrollwheels, Dropdowns, Background, CurrentWeapon, Health</t>
+  </si>
+  <si>
+    <t>Sakura Tree, TR BonsaiTree, StreetTrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SewageFloor, GarbageCans, Benches, DragonStatues, Bushes, TrafficSigns, StopSigns, Treeleaves, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alert, Door, Clock, Katana Use/Hit, Charge, Climbing, Finisher, Background, Wind, </t>
+  </si>
+  <si>
+    <t>HUD, Checkpoints, Respawn, FastTravel, Swimming, WaterGoingUp, SoundController, ParticleController, StatManager, QualityManager,</t>
   </si>
 </sst>
 </file>
@@ -677,7 +689,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -901,7 +913,7 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -924,7 +936,7 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -947,7 +959,7 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -966,7 +978,9 @@
       <c r="D12" s="14"/>
       <c r="E12" s="22"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -984,7 +998,9 @@
       <c r="D13" s="14"/>
       <c r="E13" s="22"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1002,7 +1018,9 @@
       <c r="D14" s="14"/>
       <c r="E14" s="22"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1023,7 +1041,7 @@
         <v>24</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1042,7 +1060,9 @@
       <c r="D16" s="14"/>
       <c r="E16" s="22"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1063,7 +1083,7 @@
         <v>25</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1083,7 +1103,7 @@
       <c r="E18" s="22"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1141,7 +1161,7 @@
         <v>26</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1161,7 +1181,7 @@
       <c r="E22" s="22"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1183,7 +1203,7 @@
         <v>27</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>

</xml_diff>

<commit_message>
Asset list af voor nu
</commit_message>
<xml_diff>
--- a/Algemeen/Asset_List_Ninja_Breakout.xlsx
+++ b/Algemeen/Asset_List_Ninja_Breakout.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ID Code</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>HUD, Checkpoints, Respawn, FastTravel, Swimming, WaterGoingUp, SoundController, ParticleController, StatManager, QualityManager,</t>
+  </si>
+  <si>
+    <t>GameManager, SceneManager, RenderManager(?)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
   <dimension ref="A1:R593"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1122,7 +1125,9 @@
       <c r="D19" s="14"/>
       <c r="E19" s="22"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>

</xml_diff>